<commit_message>
fix: calculate export_peak as minimum of import_peak and export_total
</commit_message>
<xml_diff>
--- a/TNB ToU.xlsx
+++ b/TNB ToU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f3afe2175ac67373/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{4ED75A63-5F64-40E3-94D2-1880750602B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EBE1B13-0990-4566-A5D0-09264DECAC81}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{4ED75A63-5F64-40E3-94D2-1880750602B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4ED0C2A-50A2-664C-B367-A8973E40D0AE}"/>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="0" windowWidth="21480" windowHeight="15585" xr2:uid="{B50842EA-3E3A-4FDF-A2B9-5A208B834AC4}"/>
+    <workbookView xWindow="7420" yWindow="760" windowWidth="21480" windowHeight="15580" xr2:uid="{B50842EA-3E3A-4FDF-A2B9-5A208B834AC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;RM&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;RM&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -179,10 +179,10 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -521,16 +521,16 @@
   <dimension ref="D2:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>19</v>
       </c>
@@ -539,7 +539,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -550,7 +550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>1</v>
       </c>
@@ -561,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>20</v>
       </c>
@@ -569,7 +569,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>0</v>
       </c>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>1</v>
       </c>
@@ -593,12 +593,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>0</v>
       </c>
@@ -610,7 +610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>1</v>
       </c>
@@ -622,7 +622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>4</v>
       </c>
@@ -634,7 +634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>5</v>
       </c>
@@ -646,7 +646,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>6</v>
       </c>
@@ -658,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>7</v>
       </c>
@@ -670,22 +670,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="5">
-        <f>LOOKUP(E2+50,D34:D49,E34:E49)*E2</f>
+        <f>LOOKUP(E2,D34:D49,E34:E49)*E2</f>
         <v>-61.624999999999993</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>13</v>
       </c>
@@ -697,7 +697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>14</v>
       </c>
@@ -709,7 +709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>15</v>
       </c>
@@ -721,16 +721,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>0</v>
       </c>
@@ -742,7 +742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>1</v>
       </c>
@@ -754,7 +754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>5</v>
       </c>
@@ -766,7 +766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>6</v>
       </c>
@@ -778,25 +778,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="5">
-        <f>LOOKUP(E2+50,D34:D49,E34:E49)*-E5</f>
+        <f>LOOKUP(E2,D34:D49,E34:E49)*-E5</f>
         <v>46.98</v>
       </c>
       <c r="F28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>17</v>
       </c>
@@ -808,13 +808,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D32" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="6" t="s">
         <v>8</v>
       </c>
@@ -822,129 +822,129 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="6">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="E34" s="6">
         <v>-0.25</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="6">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="E35" s="6">
         <v>-0.245</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="6">
-        <v>300</v>
+        <v>251</v>
       </c>
       <c r="E36" s="6">
         <v>-0.22500000000000001</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" s="6">
-        <v>350</v>
+        <v>301</v>
       </c>
       <c r="E37" s="6">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" s="6">
-        <v>400</v>
+        <v>351</v>
       </c>
       <c r="E38" s="6">
         <v>-0.17</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39" s="6">
-        <v>450</v>
+        <v>401</v>
       </c>
       <c r="E39" s="6">
         <v>-0.14499999999999999</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D40" s="6">
-        <v>500</v>
+        <v>451</v>
       </c>
       <c r="E40" s="6">
         <v>-0.12</v>
       </c>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D41" s="6">
-        <v>550</v>
+        <v>501</v>
       </c>
       <c r="E41" s="6">
         <v>-0.105</v>
       </c>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D42" s="6">
-        <v>600</v>
+        <v>551</v>
       </c>
       <c r="E42" s="6">
         <v>-0.09</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D43" s="6">
-        <v>650</v>
+        <v>601</v>
       </c>
       <c r="E43" s="6">
         <v>-7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D44" s="6">
-        <v>700</v>
+        <v>651</v>
       </c>
       <c r="E44" s="6">
         <v>-5.5E-2</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D45" s="6">
-        <v>750</v>
+        <v>701</v>
       </c>
       <c r="E45" s="6">
         <v>-4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D46" s="6">
-        <v>800</v>
+        <v>751</v>
       </c>
       <c r="E46" s="6">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D47" s="6">
-        <v>850</v>
+        <v>801</v>
       </c>
       <c r="E47" s="6">
         <v>-2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D48" s="6">
-        <v>900</v>
+        <v>851</v>
       </c>
       <c r="E48" s="6">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D49" s="6">
-        <v>1000</v>
+        <v>901</v>
       </c>
       <c r="E49" s="6">
         <v>-5.0000000000000001E-3</v>

</xml_diff>